<commit_message>
Se agrego la matriz de comunicación y de responsables a las carpetas correspondientes
</commit_message>
<xml_diff>
--- a/INTyADMIN/Plaeación del proyecto/Matriz de responsabilidades/Matriz de responsabilidades.xlsx
+++ b/INTyADMIN/Plaeación del proyecto/Matriz de responsabilidades/Matriz de responsabilidades.xlsx
@@ -8,57 +8,48 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Proyecto\v2 SSH\Aplicaci-n-para-control-de-cursos-de-capacitaci-n\INTyADMIN\Plaeación del proyecto\Matriz de responsabilidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47FDE1F-6FC6-44C5-B0B6-D4E68FDDDA42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7C2E45-A1A2-43D6-979E-F69D1318230F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identificación" sheetId="1" r:id="rId1"/>
     <sheet name="Cambios" sheetId="3" r:id="rId2"/>
     <sheet name="Matriz de reponsabilidades" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="72">
   <si>
     <t>&lt;Logotipo&gt;</t>
   </si>
   <si>
-    <t>&lt;Titulo del documento&gt;</t>
-  </si>
-  <si>
     <t>Versión</t>
   </si>
   <si>
-    <t>[x.x]</t>
-  </si>
-  <si>
     <t>Proyecto</t>
   </si>
   <si>
-    <t>[Nombre del Proyecto]</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
-    <t>[Fecha Revisión]</t>
-  </si>
-  <si>
     <t>Elaborado por</t>
   </si>
   <si>
-    <t>[Responsable]</t>
-  </si>
-  <si>
     <t>Localización del Documento</t>
   </si>
   <si>
@@ -219,6 +210,45 @@
   </si>
   <si>
     <t>[1.0]</t>
+  </si>
+  <si>
+    <t>Aplicación para control de cursos de capacitación</t>
+  </si>
+  <si>
+    <t>Jorge Luis Troncoso Camacho</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>JLTM</t>
+  </si>
+  <si>
+    <t>Se inicio la matriz de responzanbilidades pero se dejo en un 30 % terminada.</t>
+  </si>
+  <si>
+    <t>Se modifico la Matríz y se completo con las todas las faces y actividades.</t>
+  </si>
+  <si>
+    <t>MACO</t>
+  </si>
+  <si>
+    <t>Líder de proyecto</t>
+  </si>
+  <si>
+    <t>Admin de la config.</t>
+  </si>
+  <si>
+    <t>&lt;Matríz de Responsabilidades&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Matríz de Responsabilidades</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>[1.1]</t>
   </si>
 </sst>
 </file>
@@ -441,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -483,6 +513,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -495,32 +531,44 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,6 +585,114 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>42563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B2B963D-270D-4F07-B657-2408FD3898FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="5796" b="10641"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="466725" y="152400"/>
+          <a:ext cx="1276350" cy="842663"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>80663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EE19C46-B69E-4ADB-A978-8761703420FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="5796" b="10641"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="323850" y="0"/>
+          <a:ext cx="1276350" cy="842663"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -804,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,21 +978,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="17"/>
+      <c r="B3" s="19"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="17"/>
+      <c r="B5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -844,7 +1000,7 @@
     <row r="7" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -854,10 +1010,10 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -865,19 +1021,21 @@
     <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="C11" s="32">
+        <v>44049</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -885,10 +1043,10 @@
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -896,10 +1054,10 @@
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -907,10 +1065,10 @@
     <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="5"/>
@@ -924,42 +1082,54 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="19"/>
+      <c r="B16" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="21"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="35">
+        <v>44016</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="35">
+        <v>44042</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="35">
+        <v>44049</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
@@ -972,42 +1142,54 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="19"/>
+      <c r="B22" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="21"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="35">
+        <v>44016</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="35">
+        <v>44042</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="35">
+        <v>44049</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
@@ -1020,41 +1202,57 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="19"/>
+      <c r="B28" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="21"/>
     </row>
     <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="34">
+        <v>44016</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="B31" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="34">
+        <v>44042</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
@@ -1071,6 +1269,7 @@
     <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1078,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,22 +1289,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
+      <c r="A2" s="19"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="19"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="19"/>
     </row>
     <row r="6" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,61 +1312,59 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="B10" s="32">
+        <v>44049</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
     </row>
@@ -1184,38 +1381,54 @@
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="34">
+        <v>44016</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="34">
+        <v>44042</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
@@ -1229,15 +1442,16 @@
     <mergeCell ref="A16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,63 +1462,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>49</v>
-      </c>
       <c r="J1" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1319,546 +1533,554 @@
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="29"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="29"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="31"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="31"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="31"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="31"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="J8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="B20" s="31"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="22"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="22"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="22"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="22"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="22"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="22"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
+      <c r="B21" s="31"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="31"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="31"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="31"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="31"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="31"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="22"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="31"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="22"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="31"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="31"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="31"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="22"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="22"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="31"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="22"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="31"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="22"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="31"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
-      <c r="B37" s="22"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="31"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="31"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="31"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="22"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="31"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="22"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="31"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" s="22"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="31"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="31"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="31"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="31"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="31"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
-      <c r="B47" s="22"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="31"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
-      <c r="B48" s="22"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="31"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
-      <c r="B49" s="22"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="31"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="31"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
-      <c r="B51" s="22"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="31"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="22"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="31"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="21"/>
-      <c r="B53" s="22"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="31"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="21"/>
-      <c r="B54" s="22"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="31"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
-      <c r="B55" s="22"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="31"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="21"/>
-      <c r="B56" s="22"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="31"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
-      <c r="B57" s="22"/>
+      <c r="A57" s="30"/>
+      <c r="B57" s="31"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="21"/>
-      <c r="B58" s="22"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="31"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
-      <c r="B59" s="22"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="31"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
-      <c r="B60" s="22"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="31"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="21"/>
-      <c r="B61" s="22"/>
+      <c r="A61" s="30"/>
+      <c r="B61" s="31"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="21"/>
-      <c r="B62" s="22"/>
+      <c r="A62" s="30"/>
+      <c r="B62" s="31"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="21"/>
-      <c r="B63" s="22"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="31"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="21"/>
-      <c r="B64" s="22"/>
+      <c r="A64" s="30"/>
+      <c r="B64" s="31"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="21"/>
-      <c r="B65" s="22"/>
+      <c r="A65" s="30"/>
+      <c r="B65" s="31"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="21"/>
-      <c r="B66" s="22"/>
+      <c r="A66" s="30"/>
+      <c r="B66" s="31"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="21"/>
-      <c r="B67" s="22"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="31"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="21"/>
-      <c r="B68" s="22"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="31"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="21"/>
-      <c r="B69" s="22"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="31"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="30"/>
+      <c r="B70" s="31"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="26"/>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B72" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B73" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="31"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="26"/>
     </row>
     <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C74" s="23"/>
       <c r="D74" s="23"/>
     </row>
     <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C75" s="23"/>
       <c r="D75" s="23"/>
     </row>
+    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+    </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B72:D72"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>